<commit_message>
StyleMerger Use Copy Of baseStyle
Using baseStyle directly can lead to the by-reference problems associated with Cell and Style.
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/issue.4539.xlsx
+++ b/tests/data/Reader/XLSX/issue.4539.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ccchapman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6837B2BA-83B1-4C40-902E-EFF2772C9DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884986C-A26A-4354-AED0-B673C72E765E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="660" windowWidth="25440" windowHeight="15320" xr2:uid="{65964D0D-CF33-E045-A72D-D4556C030856}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{65964D0D-CF33-E045-A72D-D4556C030856}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -88,7 +89,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <border>
+        <top style="thin">
+          <color rgb="FF92D050"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color rgb="FFFF0000"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -418,55 +442,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1DD2EC-1E2F-DC4B-A8B1-9C34C93B08E8}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A7">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -477,6 +514,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A11:A13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{4ca0b373-e9b1-4578-8e53-53d6aaa79771}" enabled="1" method="Standard" siteId="{f9465cb1-7889-4d9a-b552-fdd0addf0eb1}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>